<commit_message>
udpates january, 11, 2019
</commit_message>
<xml_diff>
--- a/Totally accurate natural disaster simulator info.xlsx
+++ b/Totally accurate natural disaster simulator info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leon\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Da-Hong Setoo\Documents\GitHub\project-lanoflatfaceo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55AAFF09-2AB1-4674-9879-AA68F34E4A8F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8930867-AA6D-4F33-A35F-A91F3036A574}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{0A7432FE-FCC4-4122-BC3C-0721823B724E}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -466,7 +465,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>